<commit_message>
Linkedin courses update - BIM + Cyber + Construction
</commit_message>
<xml_diff>
--- a/0_CERTIFICATES/2024-08-26_COURSE_Sheet.xlsx
+++ b/0_CERTIFICATES/2024-08-26_COURSE_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\0_CERTIFICATES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4E9107-7492-4A54-AD87-3C1C40CFCC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B4CE17-6ADD-4BEB-B5B3-EC00FCA1447F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CourseraPlus_01" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CourseraPlus_01!$B$4:$H$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">LinkedIn_Learning!$B$4:$G$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Old_REF!$B$4:$H$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">CourseraPlus_01!$A$1:$H$24</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Old_REF!$A$1:$H$22</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="176">
   <si>
     <t>COURSERA Plus Courses</t>
   </si>
@@ -550,6 +551,27 @@
   </si>
   <si>
     <t>Applied Cybersecurity Ethics Privacy AI and Emerging Threats</t>
+  </si>
+  <si>
+    <t>2025 - 03 - 19</t>
+  </si>
+  <si>
+    <t>Construction Management Foundations</t>
+  </si>
+  <si>
+    <t>2025 - 01 - 05</t>
+  </si>
+  <si>
+    <t>2025 - 01 - 06</t>
+  </si>
+  <si>
+    <t>Construction Management Managing Risk</t>
+  </si>
+  <si>
+    <t>Transitioning to a Career in Cybersecurity</t>
+  </si>
+  <si>
+    <t>BIM Manager Managing CAD Standards</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1158,7 @@
   </sheetPr>
   <dimension ref="B1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -3157,10 +3179,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B2:I30"/>
+  <dimension ref="B2:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3193,7 +3215,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3294,7 +3316,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="16">
-        <f t="shared" ref="B9:B30" ca="1" si="1">IFERROR(OFFSET(B9,-1,0,1,1)+1,"")</f>
+        <f t="shared" ref="B9:B34" ca="1" si="1">IFERROR(OFFSET(B9,-1,0,1,1)+1,"")</f>
         <v>5</v>
       </c>
       <c r="C9" s="17" t="s">
@@ -3718,7 +3740,84 @@
       </c>
       <c r="G30" s="23"/>
     </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="16">
+        <f t="shared" ca="1" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="F31" s="20">
+        <v>2025</v>
+      </c>
+      <c r="G31" s="23"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="16">
+        <f t="shared" ca="1" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="F32" s="20">
+        <v>2025</v>
+      </c>
+      <c r="G32" s="23"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="16">
+        <f t="shared" ca="1" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="F33" s="20">
+        <v>2025</v>
+      </c>
+      <c r="G33" s="23"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="16">
+        <f t="shared" ca="1" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="F34" s="20">
+        <v>2025</v>
+      </c>
+      <c r="G34" s="23"/>
+    </row>
   </sheetData>
+  <autoFilter ref="B4:G34" xr:uid="{630D6B9D-C5F0-4332-9319-D6CA83C18678}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>